<commit_message>
Sprint 5 Unidad 2
</commit_message>
<xml_diff>
--- a/03_Data_Analysis/Sprint_05/Unidad_02_Procesado_Datos_Internos_Ficheros/02_Ejercicios_Workout/data/ejercicio_excel.xlsx
+++ b/03_Data_Analysis/Sprint_05/Unidad_02_Procesado_Datos_Internos_Ficheros/02_Ejercicios_Workout/data/ejercicio_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,212 +434,251 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>año</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>acontecimiento</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>lugar</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
         <v>1993</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>La creación de la Unión Europea</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Europa</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
         <v>1989</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>La caída del Muro de Berlín</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Alemania</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
         <v>1953</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>La primera ascensión al Everest</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Nepal/China</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
         <v>1949</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>La creación de la República Popular China</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>China</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
         <v>1947</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>La independencia de la India</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>India</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
         <v>1945</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>El final de la Segunda Guerra Mundial</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>el Mundo</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
         <v>1944</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>La invasión de Normandía durante la Segunda Guerra Mundial</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Francia</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
         <v>1928</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>El descubrimiento de la penicilina por Alexander Fleming</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Reino Unido</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
         <v>1919</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>La firma del Tratado de Versalles</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Francia</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
         <v>1917</v>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>La Revolución Rusa</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>Rusia</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
         <v>1914</v>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>El inicio de la Primera Guerra Mundial</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>Europa</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
         <v>1912</v>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>El hundimiento del Titanic</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>el Atlántico Norte</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
         <v>1903</v>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>El primer vuelo de los hermanos Wright</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>Estados Unidos</t>
         </is>

</xml_diff>